<commit_message>
Update Past Winning Notebooks.xlsx
</commit_message>
<xml_diff>
--- a/Kaggle ML & DS Survey/Past Winning Notebooks.xlsx
+++ b/Kaggle ML & DS Survey/Past Winning Notebooks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bohao/Documents/GitHub/Personal-Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bohao/Documents/GitHub/Personal-Projects/Kaggle ML &amp; DS Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9683BDB-106C-5545-AA1F-A4EDD357D325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A2B6F7-EB09-054B-B577-5F30408243E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23760" yWindow="9160" windowWidth="24920" windowHeight="17440" xr2:uid="{58E96EF9-3CB6-854E-9BC4-D787E2D265C8}"/>
+    <workbookView xWindow="21880" yWindow="9380" windowWidth="24920" windowHeight="17440" xr2:uid="{58E96EF9-3CB6-854E-9BC4-D787E2D265C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,17 +129,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="TimesNewRomanPSMT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
       <name val="TimesNewRomanPSMT"/>
       <family val="2"/>
     </font>
@@ -161,9 +154,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -173,12 +165,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,7 +485,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -520,7 +511,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>2021</v>
       </c>
@@ -528,31 +519,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21">
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21">
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21">
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>2020</v>
       </c>
@@ -560,37 +551,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>2019</v>
       </c>
@@ -598,37 +589,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21">
+    <row r="17" spans="1:2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21">
+    <row r="18" spans="1:2">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21">
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>2018</v>
       </c>
@@ -636,37 +627,37 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="21">
+    <row r="20" spans="1:2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="21">
+    <row r="21" spans="1:2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="21">
+    <row r="22" spans="1:2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21">
+    <row r="23" spans="1:2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21">
+    <row r="24" spans="1:2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="21">
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>2017</v>
       </c>
@@ -674,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="21">
+    <row r="26" spans="1:2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
         <v>25</v>
@@ -688,33 +679,6 @@
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A26"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8BCF29F0-3238-E54E-8628-96FC70827EC4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{05FBE0C0-791B-9E43-9411-4BB392E3BE5A}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{4FA4080E-A735-A84F-9234-8436F98667DC}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E7C682BB-E4A7-234F-8436-794741DAFCF7}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{B73F174D-B482-4843-AB08-EA06C777853E}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{95D23D8A-F582-714B-B754-616803A10B3C}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{FCC69F31-38CA-5745-9640-460490A6145D}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{EE8BC2E7-6351-5B43-8737-C87E03B9415B}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{7970C5B1-A5B9-034D-B0F1-26F18F5331E5}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{D79FBF4E-6919-C54C-A672-D6A3F2C8CC89}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{4BCD3F2C-7C0A-6F46-B787-8FF1F1B73DF7}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{0BCDBC79-5DFF-1A41-A263-E9F2FD8AB73E}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{34E733F0-C2D2-A747-ABB6-EF84D2B6AF76}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{D9ECB453-8C48-194D-96C2-7F769D654145}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{B43E4120-D054-0F47-AA21-7AD77BF06CDF}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{DDEE210F-1E05-2F4B-B8E0-C105F5BEAFEB}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{9F330655-32DC-7F45-B6E6-CE9330421BA5}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{C5B844B5-B613-8549-B539-545CAEB30C68}"/>
-    <hyperlink ref="B20" r:id="rId19" location=":~:text=A%20Tale%20of%204%20Kaggler%20Types%20by%20IDE%20use" xr:uid="{42BC9C66-B3B8-6640-8776-7118B7FCB493}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{A1594B22-7308-0440-8B65-DE524E95CBFB}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{3146A0E5-ECBD-7646-A9A6-708BCD7D1315}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{A0E224B0-ADBA-3047-A734-4FF17F23602D}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{BC66C365-A60D-3E47-9A1E-75477D143B63}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{36D11D8C-6D9D-AB47-A5BB-DD8AB0DE18C6}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{FA218190-B032-FA41-84DE-2ADF6079B54E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>